<commit_message>
[building] Add zinc and electrods
</commit_message>
<xml_diff>
--- a/support_data/data/dict_levels.xlsx
+++ b/support_data/data/dict_levels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Analytics\Илья\!repositories\price_analysis\support_data\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284AF78C-67EF-4FB9-8FCD-4A50005A604E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075BC9B4-B800-4B38-B372-1A0FAE4DBD91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="32760" windowWidth="28800" windowHeight="11925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20904" uniqueCount="5105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20928" uniqueCount="5113">
   <si>
     <t>Заклепки 4,0*12мм</t>
   </si>
@@ -15338,6 +15338,30 @@
   </si>
   <si>
     <t>Швеллер гнутый</t>
+  </si>
+  <si>
+    <t>Прочие материалы</t>
+  </si>
+  <si>
+    <t>Проволка сварочная, электроды</t>
+  </si>
+  <si>
+    <t>Электрод 50А (220552, 100552)</t>
+  </si>
+  <si>
+    <t>Электрод 200А арт.220352 (100352)</t>
+  </si>
+  <si>
+    <t>Электрод 80А (220842, 100842)</t>
+  </si>
+  <si>
+    <t>Электрод 105А (220842)</t>
+  </si>
+  <si>
+    <t>Электрод (220181, 100181)</t>
+  </si>
+  <si>
+    <t>Электрод 80А(220187)</t>
   </si>
 </sst>
 </file>
@@ -15688,10 +15712,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Лист2"/>
-  <dimension ref="A1:D5226"/>
+  <dimension ref="A1:D5232"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2955" sqref="C2955:C2964"/>
+    <sheetView tabSelected="1" topLeftCell="A5194" workbookViewId="0">
+      <selection activeCell="A5227" sqref="A5227:A5232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -88863,6 +88887,90 @@
         <v>3981</v>
       </c>
     </row>
+    <row r="5227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5227" t="s">
+        <v>5108</v>
+      </c>
+      <c r="B5227" t="s">
+        <v>5105</v>
+      </c>
+      <c r="C5227" t="s">
+        <v>5106</v>
+      </c>
+      <c r="D5227" t="s">
+        <v>1936</v>
+      </c>
+    </row>
+    <row r="5228" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5228" t="s">
+        <v>5109</v>
+      </c>
+      <c r="B5228" t="s">
+        <v>5105</v>
+      </c>
+      <c r="C5228" t="s">
+        <v>5106</v>
+      </c>
+      <c r="D5228" t="s">
+        <v>1936</v>
+      </c>
+    </row>
+    <row r="5229" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5229" t="s">
+        <v>5110</v>
+      </c>
+      <c r="B5229" t="s">
+        <v>5105</v>
+      </c>
+      <c r="C5229" t="s">
+        <v>5106</v>
+      </c>
+      <c r="D5229" t="s">
+        <v>1936</v>
+      </c>
+    </row>
+    <row r="5230" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5230" t="s">
+        <v>5111</v>
+      </c>
+      <c r="B5230" t="s">
+        <v>5105</v>
+      </c>
+      <c r="C5230" t="s">
+        <v>5106</v>
+      </c>
+      <c r="D5230" t="s">
+        <v>1936</v>
+      </c>
+    </row>
+    <row r="5231" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5231" t="s">
+        <v>5112</v>
+      </c>
+      <c r="B5231" t="s">
+        <v>5105</v>
+      </c>
+      <c r="C5231" t="s">
+        <v>5106</v>
+      </c>
+      <c r="D5231" t="s">
+        <v>1936</v>
+      </c>
+    </row>
+    <row r="5232" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5232" t="s">
+        <v>5107</v>
+      </c>
+      <c r="B5232" t="s">
+        <v>5105</v>
+      </c>
+      <c r="C5232" t="s">
+        <v>5106</v>
+      </c>
+      <c r="D5232" t="s">
+        <v>1936</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D5226" xr:uid="{7FA33AAD-C927-4B77-A017-55788A8F10AD}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>